<commit_message>
update Gantt Chart, Project Plan, and references. catchup update
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49F95A16-3EA3-41F6-B010-6382851905DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD943325-315F-4E87-A336-32C6459BBE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
   <si>
     <t>dont know yet</t>
   </si>
@@ -176,28 +176,28 @@
     <t>1 week</t>
   </si>
   <si>
-    <t xml:space="preserve">  1.1 Project Overview</t>
-  </si>
-  <si>
-    <t>1 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  1.2 Work Breakdown Structure</t>
+    <t xml:space="preserve">  1.1 Project Overview (develop project overview)</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.2 Work Breakdown Structure(formulate wbs)</t>
   </si>
   <si>
     <t>2 days</t>
   </si>
   <si>
-    <t xml:space="preserve">  1.3 Activity Definition and Estimation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  1.4 Gantt Chart</t>
+    <t xml:space="preserve">  1.3 Activity Definition and Estimation(state activity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.4 Gantt Chart(derive gantt chart from wbs)</t>
   </si>
   <si>
     <t>2. Software Design Document</t>
   </si>
   <si>
-    <t>19 days</t>
+    <t>19 days?</t>
   </si>
   <si>
     <t xml:space="preserve">  2.1 System Vision Statement</t>
@@ -206,16 +206,16 @@
     <t>6 hours</t>
   </si>
   <si>
-    <t xml:space="preserve">    2.1.1 Background </t>
+    <t xml:space="preserve">    2.1.1 Background (explain the bckgrnd)</t>
   </si>
   <si>
     <t>2 hours</t>
   </si>
   <si>
-    <t xml:space="preserve">    2.1.2 Overview</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    2.1.3 Benefits</t>
+    <t xml:space="preserve">    2.1.2 Overview(give overview of doc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.1.3 Benefits(Benefits of the Softwre)</t>
   </si>
   <si>
     <t xml:space="preserve">  2.2 Requirements</t>
@@ -224,22 +224,19 @@
     <t>3 days</t>
   </si>
   <si>
-    <t xml:space="preserve">    2.2.1 User Requirements</t>
-  </si>
-  <si>
-    <t>1 day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    2.2.2 Software Requirements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    2.2.3 Use Case Diagram</t>
+    <t xml:space="preserve">    2.2.1 User Requirements(List user reqs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.2.2 Software Requirements(List soft reqs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.2.3 Use Case Diagram(form UC diag)</t>
   </si>
   <si>
     <t>4 hours</t>
   </si>
   <si>
-    <t xml:space="preserve">    2.2.4 Use Cases</t>
+    <t xml:space="preserve">    2.2.4 Use Cases(develop use case)</t>
   </si>
   <si>
     <t xml:space="preserve">  2.3 Software Design and System Components </t>
@@ -257,13 +254,13 @@
     <t>9 days</t>
   </si>
   <si>
-    <t xml:space="preserve">       2.3.2.1 Functions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       2.3.2.2 Data Structures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       2.3.2.3 Detailed design</t>
+    <t xml:space="preserve">       2.3.2.1 Functions(List Funcs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       2.3.2.2 Data Structures(Specify data strctures)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       2.3.2.3 Detailed design(make dtailed design)</t>
   </si>
   <si>
     <t>5 days</t>
@@ -272,10 +269,10 @@
     <t xml:space="preserve">  2.4 User Interface Design</t>
   </si>
   <si>
-    <t xml:space="preserve">    2.4.1 Structural Design </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    2.4.2 Visual Design</t>
+    <t xml:space="preserve">    2.4.1 Structural Design (specify system env)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.4.2 Visual Design(formulate design elems)</t>
   </si>
   <si>
     <t>4 days</t>
@@ -290,22 +287,22 @@
     <t xml:space="preserve">  3.1 Design Implementation</t>
   </si>
   <si>
-    <t xml:space="preserve">    3.1.1 UI Design</t>
+    <t xml:space="preserve">    3.1.1 UI Design(storyboard? )</t>
   </si>
   <si>
     <t xml:space="preserve">  3.2 Code Construction</t>
   </si>
   <si>
-    <t xml:space="preserve">    3.2.1 Landing Page Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    3.2.2 Matplotlib Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    3.2.3 Tkinter Code/wxPython</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    3.2.4 Pandas Code</t>
+    <t xml:space="preserve">    3.2.1 Landing Page Code(code the Landing page)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.2.2 Matplotlib Code(code the)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.2.3 Tkinter Code/wxPython(1day only)(build layout)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.2.4 Pandas Code(code the)</t>
   </si>
   <si>
     <t>4 Software Testing Report</t>
@@ -314,16 +311,16 @@
     <t> </t>
   </si>
   <si>
-    <t xml:space="preserve">  4.1 Testing Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  4.2 Ongoing testing</t>
+    <t xml:space="preserve">  4.1 Testing Plan(formulate unit tests)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4.2 Ongoing testing(Ongoing Testing)</t>
   </si>
   <si>
     <t>????</t>
   </si>
   <si>
-    <t xml:space="preserve">  4.3 User Manual</t>
+    <t xml:space="preserve">  4.3 User Manual(Create user MAnual)</t>
   </si>
   <si>
     <t>7 days</t>
@@ -332,10 +329,10 @@
     <t>5 Executive Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">  5.1 Analysis and Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  5.2 Git_log</t>
+    <t xml:space="preserve">  5.1 Analysis and Comments(Analys and comments about the software )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  5.2 Git_log(Produce Git log report)</t>
   </si>
   <si>
     <t>1hr</t>
@@ -596,7 +593,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -718,6 +715,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -776,7 +838,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -906,6 +968,93 @@
     <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -917,33 +1066,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -967,11 +1089,11 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="65">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border>
@@ -984,16 +1106,15 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1057,15 +1178,16 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1083,16 +1205,15 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1170,6 +1291,20 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="9"/>
@@ -1183,35 +1318,22 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border>
@@ -1309,30 +1431,41 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1357,6 +1490,100 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="lightUp">
           <fgColor theme="7"/>
           <bgColor auto="1"/>
@@ -1370,6 +1597,92 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="lightUp">
           <fgColor theme="7"/>
           <bgColor theme="9" tint="0.59996337778862885"/>
@@ -1385,6 +1698,141 @@
       <fill>
         <patternFill patternType="lightUp">
           <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1412,6 +1860,132 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border>
@@ -1691,7 +2265,7 @@
   <dimension ref="A1:BO46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="BA13" sqref="BA13:BB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1718,13 +2292,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
       <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1732,37 +2306,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="49" t="s">
+      <c r="K2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="51"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="67"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="49" t="s">
+      <c r="Q2" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="51"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="67"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="53" t="s">
+      <c r="V2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="55"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="71"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="55"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="70"/>
+      <c r="AF2" s="70"/>
+      <c r="AG2" s="71"/>
       <c r="AH2" s="19"/>
       <c r="AI2" s="21" t="s">
         <v>7</v>
@@ -1776,22 +2350,22 @@
       <c r="AP2" s="22"/>
     </row>
     <row r="3" spans="1:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="63" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1818,12 +2392,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="45"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -2018,6 +2592,8 @@
       <c r="G5" s="6">
         <v>0</v>
       </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
@@ -2038,7 +2614,7 @@
       <c r="G6" s="7">
         <v>0</v>
       </c>
-      <c r="I6" s="16"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
@@ -2054,8 +2630,8 @@
       <c r="G7" s="7">
         <v>0</v>
       </c>
+      <c r="H7" s="16"/>
       <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
       <c r="L7" s="15"/>
       <c r="N7" s="15"/>
     </row>
@@ -2073,9 +2649,8 @@
       <c r="G8" s="7">
         <v>0</v>
       </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
       <c r="N8" s="15"/>
     </row>
     <row r="9" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2092,10 +2667,10 @@
       <c r="G9" s="7">
         <v>0</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="N9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="L9" s="43"/>
+      <c r="N9" s="43"/>
     </row>
     <row r="10" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
@@ -2111,24 +2686,25 @@
       <c r="G10" s="7">
         <v>0</v>
       </c>
-      <c r="J10" s="15"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="44"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="44"/>
+      <c r="W10" s="44"/>
+      <c r="X10" s="44"/>
+      <c r="Y10" s="44"/>
+      <c r="Z10" s="44"/>
+      <c r="AA10" s="44"/>
+      <c r="AB10" s="44"/>
+      <c r="AC10" s="44"/>
     </row>
     <row r="11" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
@@ -2144,7 +2720,7 @@
       <c r="G11" s="7">
         <v>0</v>
       </c>
-      <c r="L11" s="16"/>
+      <c r="K11" s="47"/>
     </row>
     <row r="12" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
@@ -2160,7 +2736,7 @@
       <c r="G12" s="7">
         <v>0</v>
       </c>
-      <c r="L12" s="16"/>
+      <c r="K12" s="46"/>
     </row>
     <row r="13" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
@@ -2176,7 +2752,7 @@
       <c r="G13" s="7">
         <v>0</v>
       </c>
-      <c r="M13" s="16"/>
+      <c r="K13" s="46"/>
     </row>
     <row r="14" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
@@ -2192,7 +2768,7 @@
       <c r="G14" s="7">
         <v>0</v>
       </c>
-      <c r="M14" s="16"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
@@ -2208,9 +2784,10 @@
       <c r="G15" s="7">
         <v>0</v>
       </c>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
     </row>
     <row r="16" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
@@ -2219,132 +2796,137 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="25" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7">
         <v>0</v>
       </c>
-      <c r="N16" s="16"/>
-    </row>
-    <row r="17" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="46"/>
+    </row>
+    <row r="17" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="25" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7">
         <v>0</v>
       </c>
-      <c r="O17" s="16"/>
-    </row>
-    <row r="18" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="46"/>
+    </row>
+    <row r="18" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="7">
         <v>0</v>
       </c>
-      <c r="P18" s="16"/>
-    </row>
-    <row r="19" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="46"/>
+    </row>
+    <row r="19" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
       <c r="B19" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="25" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7">
         <v>0</v>
       </c>
-      <c r="Q19" s="16"/>
-    </row>
-    <row r="20" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+    </row>
+    <row r="20" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7">
         <v>0</v>
       </c>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="47"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="47"/>
+      <c r="V20" s="47"/>
+      <c r="W20" s="47"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="16"/>
       <c r="Z20" s="16"/>
     </row>
-    <row r="21" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="25" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7">
         <v>0</v>
       </c>
-      <c r="Q21" s="16"/>
-    </row>
-    <row r="22" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="46"/>
+    </row>
+    <row r="22" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="7">
         <v>0</v>
       </c>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="46"/>
+      <c r="U22" s="46"/>
+      <c r="V22" s="46"/>
+      <c r="W22" s="46"/>
       <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
       <c r="Z22" s="16"/>
     </row>
-    <row r="23" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="25" t="s">
@@ -2355,13 +2937,15 @@
       <c r="G23" s="7">
         <v>0</v>
       </c>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-    </row>
-    <row r="24" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="51"/>
+    </row>
+    <row r="24" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="25" t="s">
@@ -2372,116 +2956,123 @@
       <c r="G24" s="7">
         <v>0</v>
       </c>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-    </row>
-    <row r="25" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O24" s="50"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="50"/>
+    </row>
+    <row r="25" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="7">
         <v>0</v>
       </c>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="16"/>
-      <c r="Y25" s="16"/>
-      <c r="Z25" s="16"/>
-    </row>
-    <row r="26" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+    </row>
+    <row r="26" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="7">
         <v>0</v>
       </c>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="16"/>
-      <c r="AC26" s="16"/>
-      <c r="AD26" s="16"/>
-      <c r="AE26" s="16"/>
-    </row>
-    <row r="27" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
+      <c r="AC26" s="1"/>
+      <c r="AE26" s="1"/>
+    </row>
+    <row r="27" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="25" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="7">
         <v>0</v>
       </c>
-      <c r="AA27" s="16"/>
-    </row>
-    <row r="28" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O27" s="46"/>
+    </row>
+    <row r="28" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="7">
         <v>0</v>
       </c>
-      <c r="AB28" s="16"/>
-      <c r="AC28" s="16"/>
-      <c r="AD28" s="16"/>
-      <c r="AE28" s="16"/>
-    </row>
-    <row r="29" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="AC28" s="1"/>
+      <c r="AE28" s="1"/>
+    </row>
+    <row r="29" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="7">
         <v>0</v>
       </c>
-      <c r="AF29" s="16"/>
-      <c r="AG29" s="16"/>
-      <c r="AH29" s="16"/>
-      <c r="AI29" s="16"/>
-      <c r="AJ29" s="16"/>
-      <c r="AK29" s="16"/>
-      <c r="AL29" s="16"/>
-      <c r="AM29" s="16"/>
-      <c r="AN29" s="16"/>
-      <c r="AO29" s="16"/>
-      <c r="AP29" s="16"/>
-      <c r="AQ29" s="16"/>
-      <c r="AR29" s="16"/>
-    </row>
-    <row r="30" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X29" s="54"/>
+      <c r="Y29" s="54"/>
+      <c r="Z29" s="54"/>
+      <c r="AA29" s="52"/>
+      <c r="AB29" s="52"/>
+      <c r="AC29" s="52"/>
+      <c r="AD29" s="52"/>
+      <c r="AE29" s="52"/>
+      <c r="AF29" s="52"/>
+      <c r="AG29" s="52"/>
+      <c r="AH29" s="52"/>
+      <c r="AI29" s="52"/>
+      <c r="AJ29" s="52"/>
+    </row>
+    <row r="30" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="25" t="s">
@@ -2492,14 +3083,14 @@
       <c r="G30" s="7">
         <v>0</v>
       </c>
-      <c r="AF30" s="16"/>
-      <c r="AG30" s="16"/>
-      <c r="AH30" s="16"/>
-    </row>
-    <row r="31" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X30" s="56"/>
+      <c r="Y30" s="56"/>
+      <c r="Z30" s="56"/>
+    </row>
+    <row r="31" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="25" t="s">
@@ -2510,58 +3101,59 @@
       <c r="G31" s="7">
         <v>0</v>
       </c>
-      <c r="AF31" s="16"/>
-      <c r="AG31" s="16"/>
-      <c r="AH31" s="16"/>
-    </row>
-    <row r="32" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X31" s="55"/>
+      <c r="Y31" s="55"/>
+      <c r="Z31" s="55"/>
+    </row>
+    <row r="32" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="7">
         <v>0</v>
       </c>
-      <c r="AI32" s="16"/>
-      <c r="AJ32" s="16"/>
-      <c r="AK32" s="16"/>
-      <c r="AL32" s="16"/>
-      <c r="AM32" s="16"/>
-      <c r="AN32" s="16"/>
-      <c r="AO32" s="16"/>
-      <c r="AP32" s="16"/>
-      <c r="AQ32" s="16"/>
-      <c r="AR32" s="16"/>
-    </row>
-    <row r="33" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z32" s="57"/>
+      <c r="AA32" s="56"/>
+      <c r="AB32" s="56"/>
+      <c r="AC32" s="56"/>
+      <c r="AD32" s="53"/>
+      <c r="AE32" s="53"/>
+      <c r="AF32" s="53"/>
+      <c r="AG32" s="53"/>
+      <c r="AH32" s="53"/>
+      <c r="AI32" s="53"/>
+    </row>
+    <row r="33" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="7">
         <v>0</v>
       </c>
-      <c r="AI33" s="16"/>
-      <c r="AJ33" s="16"/>
-      <c r="AK33" s="16"/>
-      <c r="AL33" s="16"/>
-    </row>
-    <row r="34" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA33" s="55"/>
+      <c r="AB33" s="55"/>
+      <c r="AC33" s="55"/>
+      <c r="AD33" s="55"/>
+      <c r="AE33" s="55"/>
+    </row>
+    <row r="34" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="25" t="s">
@@ -2572,14 +3164,14 @@
       <c r="G34" s="7">
         <v>0</v>
       </c>
-      <c r="AL34" s="16"/>
-      <c r="AM34" s="16"/>
-      <c r="AN34" s="16"/>
-    </row>
-    <row r="35" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA34" s="55"/>
+      <c r="AB34" s="55"/>
+      <c r="AC34" s="55"/>
+    </row>
+    <row r="35" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="25" t="s">
@@ -2590,14 +3182,12 @@
       <c r="G35" s="7">
         <v>0</v>
       </c>
-      <c r="AN35" s="16"/>
-      <c r="AO35" s="16"/>
-      <c r="AP35" s="16"/>
-    </row>
-    <row r="36" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA35" s="55"/>
+    </row>
+    <row r="36" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>32</v>
@@ -2605,97 +3195,102 @@
       <c r="G36" s="7">
         <v>0</v>
       </c>
-      <c r="AP36" s="16"/>
-      <c r="AQ36" s="16"/>
-      <c r="AR36" s="16"/>
-    </row>
-    <row r="37" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB36" s="55"/>
+      <c r="AC36" s="55"/>
+      <c r="AD36" s="55"/>
+      <c r="AE36" s="55"/>
+    </row>
+    <row r="37" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
       <c r="B37" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="25" t="s">
-        <v>62</v>
-      </c>
       <c r="G37" s="7">
         <v>0</v>
       </c>
-      <c r="AS37" s="16"/>
-      <c r="AT37" s="16"/>
-      <c r="AU37" s="16"/>
-      <c r="AV37" s="16"/>
-      <c r="AW37" s="16"/>
-      <c r="AX37" s="16"/>
-      <c r="AY37" s="16"/>
-      <c r="AZ37" s="16"/>
-      <c r="BA37" s="16"/>
-      <c r="BB37" s="16"/>
-      <c r="BC37" s="16"/>
-    </row>
-    <row r="38" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25"/>
       <c r="B38" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G38" s="7">
         <v>0</v>
       </c>
-      <c r="AS38" s="16"/>
-      <c r="AT38" s="16"/>
-      <c r="AU38" s="16"/>
-      <c r="AV38" s="16"/>
-      <c r="AW38" s="16"/>
-    </row>
-    <row r="39" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA38" s="60"/>
+      <c r="AB38" s="58"/>
+      <c r="AC38" s="58"/>
+      <c r="AD38" s="58"/>
+      <c r="AE38" s="58"/>
+      <c r="AF38" s="58"/>
+    </row>
+    <row r="39" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
       <c r="B39" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="25" t="s">
-        <v>65</v>
-      </c>
       <c r="G39" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB39" s="59"/>
+      <c r="AC39" s="59"/>
+      <c r="AD39" s="59"/>
+      <c r="AE39" s="59"/>
+      <c r="AF39" s="59"/>
+    </row>
+    <row r="40" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D40" s="25" t="s">
-        <v>67</v>
-      </c>
       <c r="G40" s="7">
         <v>0</v>
       </c>
-      <c r="AW40" s="16"/>
-      <c r="AX40" s="16"/>
-      <c r="AY40" s="16"/>
-      <c r="AZ40" s="16"/>
-      <c r="BA40" s="16"/>
-      <c r="BB40" s="16"/>
-      <c r="BC40" s="16"/>
-    </row>
-    <row r="41" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA40" s="59"/>
+      <c r="AB40" s="59"/>
+      <c r="AC40" s="59"/>
+      <c r="AD40" s="59"/>
+      <c r="AE40" s="59"/>
+      <c r="AF40" s="59"/>
+      <c r="AG40" s="59"/>
+      <c r="AH40" s="59"/>
+      <c r="AI40" s="59"/>
+    </row>
+    <row r="41" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
       <c r="B41" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G41" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA41" s="59"/>
+      <c r="AB41" s="59"/>
+      <c r="AC41" s="59"/>
+      <c r="AD41" s="59"/>
+      <c r="AE41" s="59"/>
+      <c r="AF41" s="59"/>
+      <c r="AG41" s="59"/>
+    </row>
+    <row r="42" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25"/>
       <c r="B42" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>32</v>
@@ -2703,165 +3298,322 @@
       <c r="G42" s="7">
         <v>0</v>
       </c>
-      <c r="BD42" s="16"/>
-      <c r="BE42" s="16"/>
-      <c r="BF42" s="16"/>
-    </row>
-    <row r="43" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA42" s="61"/>
+      <c r="AB42" s="61"/>
+      <c r="AC42" s="61"/>
+      <c r="AD42" s="61"/>
+      <c r="AE42" s="61"/>
+      <c r="AF42" s="61"/>
+      <c r="AG42" s="61"/>
+      <c r="AH42" s="61"/>
+      <c r="AI42" s="61"/>
+      <c r="AJ42" s="61"/>
+      <c r="AK42" s="61"/>
+      <c r="AL42" s="61"/>
+      <c r="AM42" s="61"/>
+    </row>
+    <row r="43" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25"/>
       <c r="B43" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="25" t="s">
+      <c r="G43" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="62"/>
+      <c r="AB43" s="62"/>
+      <c r="AC43" s="62"/>
+      <c r="AD43" s="62"/>
+      <c r="AE43" s="62"/>
+      <c r="AF43" s="62"/>
+      <c r="AG43" s="62"/>
+      <c r="AH43" s="62"/>
+      <c r="AI43" s="62"/>
+      <c r="AJ43" s="62"/>
+      <c r="AK43" s="62"/>
+      <c r="AL43" s="62"/>
+      <c r="AM43" s="62"/>
+    </row>
+    <row r="44" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="7">
+        <v>0</v>
+      </c>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
+      <c r="R44" s="62"/>
+      <c r="S44" s="62"/>
+      <c r="T44" s="62"/>
+      <c r="U44" s="62"/>
+      <c r="V44" s="62"/>
+      <c r="W44" s="62"/>
+      <c r="X44" s="62"/>
+      <c r="Y44" s="62"/>
+      <c r="Z44" s="62"/>
+      <c r="AA44" s="62"/>
+      <c r="AB44" s="62"/>
+      <c r="AC44" s="62"/>
+      <c r="AD44" s="62"/>
+      <c r="AE44" s="62"/>
+      <c r="AF44" s="62"/>
+      <c r="AG44" s="62"/>
+      <c r="AH44" s="62"/>
+      <c r="AI44" s="62"/>
+      <c r="AJ44" s="62"/>
+      <c r="AK44" s="62"/>
+      <c r="AL44" s="62"/>
+      <c r="AM44" s="62"/>
+    </row>
+    <row r="45" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G43" s="7">
-        <v>0</v>
-      </c>
-      <c r="BG43" s="16"/>
-    </row>
-    <row r="44" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G44" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="23" t="s">
-        <v>72</v>
-      </c>
       <c r="G45" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:59" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G46" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="32" priority="32">
+    <cfRule type="expression" dxfId="64" priority="144">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O5:BO5 J6:BO6 O7:BO9 K7 M7:M9 H7:H8 H9:I10 AC10:BO10 H11:K12 M11:BO12 H13:L15 N13:BO14 O16:BO16 H16:M16 H17:N17 P17:BO17 H18:O18 Q18:BO18 R19:BO19 AA20:BO20 H19:P21 R21:BO21 AA22:BO22 H22:Q23 T23:BO23 H24:S24 V24:BO24 AA25:BO25 H25:U25 K10 AF26:BO26 H26:Z27 AB27:BO27 H28:AA28 AF28:BO28 AS29:BO29 H29:AE31 AI30:BO31 P15:BO15 AS32:BO32 H32:AH33 AM33:BO33 H34:AK34 AO34:BO34 H35:AM35 AQ35:BO35 H36:AO36 AS36:BO36 H39:BO39 H37:AR38 AX38:BO38 H41:BO41 H40:AV40 BD40:BO40 BD37:BO37 H44:BO46 H42:BC42 BG42:BO42 H43:BF43 BH43:BO43">
-    <cfRule type="expression" dxfId="31" priority="25">
+  <conditionalFormatting sqref="O5:BO5 I6 K6:BO6 K7 M7:M9 O7:BO9 J8:K8 H9 K9 AD10:BO10 H10:J16 L11:BO14 O15:BO17 L16:N16 H17:K17 M17:N17 N18:BO18 H18:L19 O19:BO19 AA20:BO20 H20:M21 O21:BO21 AA22:BO22 H22:N23 Q23 S23:BO23 H24:O24 R24:BO24 AA25:BO25 H25:N29 AA26:AB28 P27:Z27 S28:Z28 AO28:BO28 AK28:AK33 AM28:AM34 O29:W29 AO29:AO35 AP29:AQ36 AS29:BO36 AR29:AR37 H30:W31 H32:Y32 AJ32 AF33:AJ33 H33:Z35 AD34:AL34 AB35:AN35 H36:AA36 AF36:AO36 H37:AQ37 AS37:AV39 AW37:BO40 AG38:AR39 H38:Z43 AJ40:AV40 AH41:BO41 AN42:BO44 H44 H45:BO46">
+    <cfRule type="expression" dxfId="63" priority="142">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="143">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="147">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="148">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="141">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="140">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="139">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="137">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="27">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T25:Z26">
+    <cfRule type="expression" dxfId="55" priority="76">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="73">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="74">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="52" priority="75">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="51" priority="80">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="79">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="78">
+      <formula>T$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="77">
+      <formula>Plan</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y20">
+    <cfRule type="expression" dxfId="47" priority="99">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="104">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="103">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="102">
+      <formula>Y$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="101">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="100">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="30">
+    <cfRule type="expression" dxfId="41" priority="98">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="97">
+      <formula>PercentComplete</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y22">
+    <cfRule type="expression" dxfId="39" priority="90">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="89">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="95">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="94">
+      <formula>Y$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="93">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="31">
-      <formula>H$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="35">
+    <cfRule type="expression" dxfId="34" priority="92">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="91">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="96">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA39">
+    <cfRule type="expression" dxfId="31" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="36">
+    <cfRule type="expression" dxfId="27" priority="6">
+      <formula>AA$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA30:AJ31">
+    <cfRule type="expression" dxfId="23" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="14">
+      <formula>AA$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="16" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H6">
-    <cfRule type="expression" dxfId="23" priority="17">
+  <conditionalFormatting sqref="AC28:AJ28">
+    <cfRule type="expression" dxfId="15" priority="58">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="64">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="59">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="60">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="61">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="62">
+      <formula>AC$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="63">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="57">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC26:BO27">
+    <cfRule type="expression" dxfId="7" priority="65">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="72">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="67">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="68">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="69">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="70">
+      <formula>AC$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="66">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="19">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="22">
-      <formula>H$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="23">
+    <cfRule type="expression" dxfId="0" priority="71">
       <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="15" priority="9">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
-      <formula>I$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>I$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
-      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
@@ -2869,8 +3621,8 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2 N7:N9 J9:J10 L7:L8" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 K9:L9 V25:Z25 J7:J8 I6:I7 K8 L10:AB10 L11:L12 M13:M15 N15:N16 O17 P18 Q19:Q21 R20:Z20 R22:Z22 R23:S23 T24:U24 AF30:AH31 AA26:AE26 AA27 AB28:AE28 AF29:AR29 J5:N5 O15 AI32:AR32 AI33:AL33 AL34:AN34 AN35:AP35 AP36:AR36 AS37:AW38 AW40:BC40 AX37:BC37 BD42:BF42 BG43" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2 N7:N9 J9 L7 L9" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 Z22 I9:L9 I7 I8:K8 H5:H8 R23 I5:N5 X20 Z20 AN35 AL34 AK32:AK33 X22" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
@@ -2899,6 +3651,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c92308a8-1835-41e9-8926-04f7d96944eb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F59D4D64CE5F8C4CA58525DF3DC0AFD5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="113e38f2615660614a99283ca940ebc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c92308a8-1835-41e9-8926-04f7d96944eb" xmlns:ns4="e356df2a-e0c9-4065-84cd-66458133e470" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5e97994a6c3a355cf6b2ac1128788" ns3:_="" ns4:_="">
     <xsd:import namespace="c92308a8-1835-41e9-8926-04f7d96944eb"/>
@@ -3119,24 +3888,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB3A5FF7-A6FB-4893-A259-58257F101003}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e356df2a-e0c9-4065-84cd-66458133e470"/>
+    <ds:schemaRef ds:uri="c92308a8-1835-41e9-8926-04f7d96944eb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c92308a8-1835-41e9-8926-04f7d96944eb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F548E22-8B9B-46C1-AC83-52672928AD7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0283A91D-6870-4AE4-8B04-308DA8D187B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3155,31 +3932,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F548E22-8B9B-46C1-AC83-52672928AD7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB3A5FF7-A6FB-4893-A259-58257F101003}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="c92308a8-1835-41e9-8926-04f7d96944eb"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e356df2a-e0c9-4065-84cd-66458133e470"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{c9f92db8-2851-4df9-9d12-fab52f5b1415}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" removed="0"/>

</xml_diff>

<commit_message>
Updated File Layouts and Finished Descriptions
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD943325-315F-4E87-A336-32C6459BBE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32934B35-5089-450A-A6F3-D8E5A9341489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,10 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
-  <si>
-    <t>dont know yet</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
   <si>
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
   </si>
@@ -287,42 +284,18 @@
     <t xml:space="preserve">  3.1 Design Implementation</t>
   </si>
   <si>
-    <t xml:space="preserve">    3.1.1 UI Design(storyboard? )</t>
-  </si>
-  <si>
     <t xml:space="preserve">  3.2 Code Construction</t>
   </si>
   <si>
-    <t xml:space="preserve">    3.2.1 Landing Page Code(code the Landing page)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    3.2.2 Matplotlib Code(code the)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    3.2.3 Tkinter Code/wxPython(1day only)(build layout)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    3.2.4 Pandas Code(code the)</t>
-  </si>
-  <si>
     <t>4 Software Testing Report</t>
   </si>
   <si>
     <t> </t>
   </si>
   <si>
-    <t xml:space="preserve">  4.1 Testing Plan(formulate unit tests)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  4.2 Ongoing testing(Ongoing Testing)</t>
-  </si>
-  <si>
     <t>????</t>
   </si>
   <si>
-    <t xml:space="preserve">  4.3 User Manual(Create user MAnual)</t>
-  </si>
-  <si>
     <t>7 days</t>
   </si>
   <si>
@@ -339,13 +312,76 @@
   </si>
   <si>
     <t>Project Completion</t>
+  </si>
+  <si>
+    <t>AJJ BNB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.1.1 Build the User Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.1.2 Place the Buttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.1.3 Add the Colours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.1.4 Build the Layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.1.4 Build the Logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.2.1 Coding: Matplotlib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.2.2 Coding: wxPython</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.2.3 Coding: Pandas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3.3 Design Integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.3.1 Coding: Landing Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.3.2 Coding: Suburn Listing Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.3.3 Coding: Price Chart Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.3.4 Coding: Search Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.3.5 Coding: Cleanliness Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.3.6 Coding: Display by Ratings Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4.1 Document Test Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4.2 Build Test Data based on test Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4.3 Perform user acceptance testing procedures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4.4 Perform user acceptance testing procedures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4.5 Perform user acceptance testing procedures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -464,6 +500,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="22">
@@ -838,7 +881,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -947,9 +990,6 @@
     <xf numFmtId="0" fontId="16" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1066,6 +1106,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -2262,10 +2308,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO46"/>
+  <dimension ref="A1:BO57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BA13" sqref="BA13:BB13"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2283,7 +2329,7 @@
   <sheetData>
     <row r="1" spans="1:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="13" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2292,54 +2338,54 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="5" t="s">
-        <v>2</v>
       </c>
       <c r="H2" s="14">
         <v>1</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="65" t="s">
+      <c r="K2" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="65" t="s">
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="69" t="s">
+      <c r="W2" s="69"/>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="70"/>
-      <c r="AF2" s="70"/>
-      <c r="AG2" s="71"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="70"/>
       <c r="AH2" s="19"/>
       <c r="AI2" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AJ2" s="22"/>
       <c r="AK2" s="22"/>
@@ -2350,26 +2396,26 @@
       <c r="AP2" s="22"/>
     </row>
     <row r="3" spans="1:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="D3" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="E3" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="F3" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="75" t="s">
+      <c r="G3" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="H3" s="20" t="s">
         <v>13</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>14</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
@@ -2392,12 +2438,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="74"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -2580,15 +2626,15 @@
       </c>
     </row>
     <row r="5" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="40" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="40"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="6">
         <v>0</v>
       </c>
@@ -2603,11 +2649,11 @@
     <row r="6" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -2619,11 +2665,11 @@
     <row r="7" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -2638,11 +2684,11 @@
     <row r="8" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2656,11 +2702,11 @@
     <row r="9" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2669,544 +2715,544 @@
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
-      <c r="L9" s="43"/>
-      <c r="N9" s="43"/>
+      <c r="L9" s="42"/>
+      <c r="N9" s="42"/>
     </row>
     <row r="10" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="41" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="42" t="s">
-        <v>24</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7">
         <v>0</v>
       </c>
-      <c r="K10" s="45"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="44"/>
-      <c r="U10" s="44"/>
-      <c r="V10" s="44"/>
-      <c r="W10" s="44"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="44"/>
-      <c r="AA10" s="44"/>
-      <c r="AB10" s="44"/>
-      <c r="AC10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="43"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
     </row>
     <row r="11" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7">
         <v>0</v>
       </c>
-      <c r="K11" s="47"/>
+      <c r="K11" s="46"/>
     </row>
     <row r="12" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
       <c r="B12" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7">
         <v>0</v>
       </c>
-      <c r="K12" s="46"/>
+      <c r="K12" s="45"/>
     </row>
     <row r="13" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="7">
         <v>0</v>
       </c>
-      <c r="K13" s="46"/>
+      <c r="K13" s="45"/>
     </row>
     <row r="14" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7">
         <v>0</v>
       </c>
-      <c r="K14" s="46"/>
+      <c r="K14" s="45"/>
     </row>
     <row r="15" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="7">
         <v>0</v>
       </c>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
     </row>
     <row r="16" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7">
         <v>0</v>
       </c>
-      <c r="K16" s="46"/>
+      <c r="K16" s="45"/>
     </row>
     <row r="17" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7">
         <v>0</v>
       </c>
-      <c r="L17" s="46"/>
+      <c r="L17" s="45"/>
     </row>
     <row r="18" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="7">
         <v>0</v>
       </c>
-      <c r="M18" s="46"/>
+      <c r="M18" s="45"/>
     </row>
     <row r="19" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
       <c r="B19" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7">
         <v>0</v>
       </c>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
     </row>
     <row r="20" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="40" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="41" t="s">
-        <v>39</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7">
         <v>0</v>
       </c>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="47"/>
-      <c r="R20" s="47"/>
-      <c r="S20" s="47"/>
-      <c r="T20" s="47"/>
-      <c r="U20" s="47"/>
-      <c r="V20" s="47"/>
-      <c r="W20" s="47"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="46"/>
       <c r="X20" s="16"/>
       <c r="Z20" s="16"/>
     </row>
     <row r="21" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7">
         <v>0</v>
       </c>
-      <c r="N21" s="46"/>
+      <c r="N21" s="45"/>
     </row>
     <row r="22" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="7">
         <v>0</v>
       </c>
-      <c r="O22" s="48"/>
-      <c r="P22" s="48"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="48"/>
-      <c r="S22" s="48"/>
-      <c r="T22" s="46"/>
-      <c r="U22" s="46"/>
-      <c r="V22" s="46"/>
-      <c r="W22" s="46"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="45"/>
       <c r="X22" s="16"/>
       <c r="Z22" s="16"/>
     </row>
     <row r="23" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7">
         <v>0</v>
       </c>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="51"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="50"/>
     </row>
     <row r="24" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="7">
         <v>0</v>
       </c>
-      <c r="O24" s="50"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="50"/>
-      <c r="S24" s="50"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
     </row>
     <row r="25" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="7">
         <v>0</v>
       </c>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="49"/>
-      <c r="R25" s="49"/>
-      <c r="S25" s="49"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="48"/>
+      <c r="S25" s="48"/>
     </row>
     <row r="26" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="7">
         <v>0</v>
       </c>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="47"/>
-      <c r="R26" s="47"/>
-      <c r="S26" s="47"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
       <c r="AC26" s="1"/>
       <c r="AE26" s="1"/>
     </row>
     <row r="27" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="7">
         <v>0</v>
       </c>
-      <c r="O27" s="46"/>
+      <c r="O27" s="45"/>
     </row>
     <row r="28" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="7">
         <v>0</v>
       </c>
-      <c r="O28" s="46"/>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
+      <c r="O28" s="45"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
       <c r="AC28" s="1"/>
       <c r="AE28" s="1"/>
     </row>
     <row r="29" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="7">
         <v>0</v>
       </c>
-      <c r="X29" s="54"/>
-      <c r="Y29" s="54"/>
-      <c r="Z29" s="54"/>
-      <c r="AA29" s="52"/>
-      <c r="AB29" s="52"/>
-      <c r="AC29" s="52"/>
-      <c r="AD29" s="52"/>
-      <c r="AE29" s="52"/>
-      <c r="AF29" s="52"/>
-      <c r="AG29" s="52"/>
-      <c r="AH29" s="52"/>
-      <c r="AI29" s="52"/>
-      <c r="AJ29" s="52"/>
+      <c r="X29" s="53"/>
+      <c r="Y29" s="53"/>
+      <c r="Z29" s="53"/>
+      <c r="AA29" s="51"/>
+      <c r="AB29" s="51"/>
+      <c r="AC29" s="51"/>
+      <c r="AD29" s="51"/>
+      <c r="AE29" s="51"/>
+      <c r="AF29" s="51"/>
+      <c r="AG29" s="51"/>
+      <c r="AH29" s="51"/>
+      <c r="AI29" s="51"/>
+      <c r="AJ29" s="51"/>
     </row>
     <row r="30" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="7">
         <v>0</v>
       </c>
-      <c r="X30" s="56"/>
-      <c r="Y30" s="56"/>
-      <c r="Z30" s="56"/>
+      <c r="X30" s="55"/>
+      <c r="Y30" s="55"/>
+      <c r="Z30" s="55"/>
     </row>
     <row r="31" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="34" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="7">
         <v>0</v>
       </c>
-      <c r="X31" s="55"/>
-      <c r="Y31" s="55"/>
-      <c r="Z31" s="55"/>
+      <c r="X31" s="54"/>
+      <c r="Y31" s="54"/>
+      <c r="Z31" s="54"/>
     </row>
     <row r="32" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
-      <c r="B32" s="33" t="s">
-        <v>55</v>
+      <c r="B32" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="7">
         <v>0</v>
       </c>
-      <c r="Z32" s="57"/>
-      <c r="AA32" s="56"/>
-      <c r="AB32" s="56"/>
-      <c r="AC32" s="56"/>
-      <c r="AD32" s="53"/>
-      <c r="AE32" s="53"/>
-      <c r="AF32" s="53"/>
-      <c r="AG32" s="53"/>
-      <c r="AH32" s="53"/>
-      <c r="AI32" s="53"/>
+      <c r="Z32" s="56"/>
+      <c r="AA32" s="55"/>
+      <c r="AB32" s="55"/>
+      <c r="AC32" s="55"/>
+      <c r="AD32" s="52"/>
+      <c r="AE32" s="52"/>
+      <c r="AF32" s="52"/>
+      <c r="AG32" s="52"/>
+      <c r="AH32" s="52"/>
+      <c r="AI32" s="52"/>
     </row>
     <row r="33" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="34" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="7">
         <v>0</v>
       </c>
-      <c r="AA33" s="55"/>
-      <c r="AB33" s="55"/>
-      <c r="AC33" s="55"/>
-      <c r="AD33" s="55"/>
-      <c r="AE33" s="55"/>
+      <c r="AA33" s="54"/>
+      <c r="AB33" s="54"/>
+      <c r="AC33" s="54"/>
+      <c r="AD33" s="54"/>
+      <c r="AE33" s="54"/>
     </row>
     <row r="34" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="34" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="7">
         <v>0</v>
       </c>
-      <c r="AA34" s="55"/>
-      <c r="AB34" s="55"/>
-      <c r="AC34" s="55"/>
+      <c r="AA34" s="54"/>
+      <c r="AB34" s="54"/>
+      <c r="AC34" s="54"/>
     </row>
     <row r="35" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="34" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="7">
         <v>0</v>
       </c>
-      <c r="AA35" s="55"/>
+      <c r="AA35" s="54"/>
     </row>
     <row r="36" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
-      <c r="B36" s="34" t="s">
-        <v>59</v>
+      <c r="B36" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G36" s="7">
         <v>0</v>
       </c>
-      <c r="AB36" s="55"/>
-      <c r="AC36" s="55"/>
-      <c r="AD36" s="55"/>
-      <c r="AE36" s="55"/>
+      <c r="AB36" s="54"/>
+      <c r="AC36" s="54"/>
+      <c r="AD36" s="54"/>
+      <c r="AE36" s="54"/>
     </row>
     <row r="37" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
-      <c r="B37" s="35" t="s">
-        <v>60</v>
+      <c r="B37" s="75" t="s">
+        <v>69</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G37" s="7">
         <v>0</v>
@@ -3214,179 +3260,237 @@
     </row>
     <row r="38" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25"/>
-      <c r="B38" s="36" t="s">
-        <v>62</v>
+      <c r="B38" s="34" t="s">
+        <v>70</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G38" s="7">
         <v>0</v>
       </c>
-      <c r="AA38" s="60"/>
-      <c r="AB38" s="58"/>
-      <c r="AC38" s="58"/>
-      <c r="AD38" s="58"/>
-      <c r="AE38" s="58"/>
-      <c r="AF38" s="58"/>
+      <c r="AA38" s="59"/>
+      <c r="AB38" s="57"/>
+      <c r="AC38" s="57"/>
+      <c r="AD38" s="57"/>
+      <c r="AE38" s="57"/>
+      <c r="AF38" s="57"/>
     </row>
     <row r="39" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
-      <c r="B39" s="36" t="s">
-        <v>63</v>
+      <c r="B39" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G39" s="7">
         <v>0</v>
       </c>
-      <c r="AB39" s="59"/>
-      <c r="AC39" s="59"/>
-      <c r="AD39" s="59"/>
-      <c r="AE39" s="59"/>
-      <c r="AF39" s="59"/>
+      <c r="AB39" s="58"/>
+      <c r="AC39" s="58"/>
+      <c r="AD39" s="58"/>
+      <c r="AE39" s="58"/>
+      <c r="AF39" s="58"/>
     </row>
     <row r="40" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
-      <c r="B40" s="36" t="s">
-        <v>65</v>
+      <c r="B40" s="33" t="s">
+        <v>72</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G40" s="7">
         <v>0</v>
       </c>
-      <c r="AA40" s="59"/>
-      <c r="AB40" s="59"/>
-      <c r="AC40" s="59"/>
-      <c r="AD40" s="59"/>
-      <c r="AE40" s="59"/>
-      <c r="AF40" s="59"/>
-      <c r="AG40" s="59"/>
-      <c r="AH40" s="59"/>
-      <c r="AI40" s="59"/>
+      <c r="AA40" s="58"/>
+      <c r="AB40" s="58"/>
+      <c r="AC40" s="58"/>
+      <c r="AD40" s="58"/>
+      <c r="AE40" s="58"/>
+      <c r="AF40" s="58"/>
+      <c r="AG40" s="58"/>
+      <c r="AH40" s="58"/>
+      <c r="AI40" s="58"/>
     </row>
     <row r="41" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
-      <c r="B41" s="37" t="s">
-        <v>67</v>
+      <c r="B41" s="75" t="s">
+        <v>73</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G41" s="7">
         <v>0</v>
       </c>
-      <c r="AA41" s="59"/>
-      <c r="AB41" s="59"/>
-      <c r="AC41" s="59"/>
-      <c r="AD41" s="59"/>
-      <c r="AE41" s="59"/>
-      <c r="AF41" s="59"/>
-      <c r="AG41" s="59"/>
+      <c r="AA41" s="58"/>
+      <c r="AB41" s="58"/>
+      <c r="AC41" s="58"/>
+      <c r="AD41" s="58"/>
+      <c r="AE41" s="58"/>
+      <c r="AF41" s="58"/>
+      <c r="AG41" s="58"/>
     </row>
     <row r="42" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25"/>
-      <c r="B42" s="38" t="s">
-        <v>68</v>
+      <c r="B42" s="75" t="s">
+        <v>74</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G42" s="7">
         <v>0</v>
       </c>
-      <c r="AA42" s="61"/>
-      <c r="AB42" s="61"/>
-      <c r="AC42" s="61"/>
-      <c r="AD42" s="61"/>
-      <c r="AE42" s="61"/>
-      <c r="AF42" s="61"/>
-      <c r="AG42" s="61"/>
-      <c r="AH42" s="61"/>
-      <c r="AI42" s="61"/>
-      <c r="AJ42" s="61"/>
-      <c r="AK42" s="61"/>
-      <c r="AL42" s="61"/>
-      <c r="AM42" s="61"/>
+      <c r="AA42" s="60"/>
+      <c r="AB42" s="60"/>
+      <c r="AC42" s="60"/>
+      <c r="AD42" s="60"/>
+      <c r="AE42" s="60"/>
+      <c r="AF42" s="60"/>
+      <c r="AG42" s="60"/>
+      <c r="AH42" s="60"/>
+      <c r="AI42" s="60"/>
+      <c r="AJ42" s="60"/>
+      <c r="AK42" s="60"/>
+      <c r="AL42" s="60"/>
+      <c r="AM42" s="60"/>
     </row>
     <row r="43" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25"/>
-      <c r="B43" s="38" t="s">
-        <v>69</v>
+      <c r="B43" s="75" t="s">
+        <v>75</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G43" s="7">
         <v>0</v>
       </c>
-      <c r="AA43" s="62"/>
-      <c r="AB43" s="62"/>
-      <c r="AC43" s="62"/>
-      <c r="AD43" s="62"/>
-      <c r="AE43" s="62"/>
-      <c r="AF43" s="62"/>
-      <c r="AG43" s="62"/>
-      <c r="AH43" s="62"/>
-      <c r="AI43" s="62"/>
-      <c r="AJ43" s="62"/>
-      <c r="AK43" s="62"/>
-      <c r="AL43" s="62"/>
-      <c r="AM43" s="62"/>
+      <c r="AA43" s="61"/>
+      <c r="AB43" s="61"/>
+      <c r="AC43" s="61"/>
+      <c r="AD43" s="61"/>
+      <c r="AE43" s="61"/>
+      <c r="AF43" s="61"/>
+      <c r="AG43" s="61"/>
+      <c r="AH43" s="61"/>
+      <c r="AI43" s="61"/>
+      <c r="AJ43" s="61"/>
+      <c r="AK43" s="61"/>
+      <c r="AL43" s="61"/>
+      <c r="AM43" s="61"/>
     </row>
     <row r="44" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="s">
-        <v>61</v>
+      <c r="B44" s="75" t="s">
+        <v>76</v>
       </c>
       <c r="G44" s="7">
         <v>0</v>
       </c>
-      <c r="I44" s="62"/>
-      <c r="J44" s="62"/>
-      <c r="K44" s="62"/>
-      <c r="L44" s="62"/>
-      <c r="M44" s="62"/>
-      <c r="N44" s="62"/>
-      <c r="O44" s="62"/>
-      <c r="P44" s="62"/>
-      <c r="Q44" s="62"/>
-      <c r="R44" s="62"/>
-      <c r="S44" s="62"/>
-      <c r="T44" s="62"/>
-      <c r="U44" s="62"/>
-      <c r="V44" s="62"/>
-      <c r="W44" s="62"/>
-      <c r="X44" s="62"/>
-      <c r="Y44" s="62"/>
-      <c r="Z44" s="62"/>
-      <c r="AA44" s="62"/>
-      <c r="AB44" s="62"/>
-      <c r="AC44" s="62"/>
-      <c r="AD44" s="62"/>
-      <c r="AE44" s="62"/>
-      <c r="AF44" s="62"/>
-      <c r="AG44" s="62"/>
-      <c r="AH44" s="62"/>
-      <c r="AI44" s="62"/>
-      <c r="AJ44" s="62"/>
-      <c r="AK44" s="62"/>
-      <c r="AL44" s="62"/>
-      <c r="AM44" s="62"/>
+      <c r="I44" s="61"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="61"/>
+      <c r="L44" s="61"/>
+      <c r="M44" s="61"/>
+      <c r="N44" s="61"/>
+      <c r="O44" s="61"/>
+      <c r="P44" s="61"/>
+      <c r="Q44" s="61"/>
+      <c r="R44" s="61"/>
+      <c r="S44" s="61"/>
+      <c r="T44" s="61"/>
+      <c r="U44" s="61"/>
+      <c r="V44" s="61"/>
+      <c r="W44" s="61"/>
+      <c r="X44" s="61"/>
+      <c r="Y44" s="61"/>
+      <c r="Z44" s="61"/>
+      <c r="AA44" s="61"/>
+      <c r="AB44" s="61"/>
+      <c r="AC44" s="61"/>
+      <c r="AD44" s="61"/>
+      <c r="AE44" s="61"/>
+      <c r="AF44" s="61"/>
+      <c r="AG44" s="61"/>
+      <c r="AH44" s="61"/>
+      <c r="AI44" s="61"/>
+      <c r="AJ44" s="61"/>
+      <c r="AK44" s="61"/>
+      <c r="AL44" s="61"/>
+      <c r="AM44" s="61"/>
     </row>
     <row r="45" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="23" t="s">
-        <v>71</v>
+      <c r="B45" s="75" t="s">
+        <v>77</v>
       </c>
       <c r="G45" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="75" t="s">
+        <v>78</v>
+      </c>
       <c r="G46" s="7">
         <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="76" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="76" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="76" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="23" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3408,7 +3512,7 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O5:BO5 I6 K6:BO6 K7 M7:M9 O7:BO9 J8:K8 H9 K9 AD10:BO10 H10:J16 L11:BO14 O15:BO17 L16:N16 H17:K17 M17:N17 N18:BO18 H18:L19 O19:BO19 AA20:BO20 H20:M21 O21:BO21 AA22:BO22 H22:N23 Q23 S23:BO23 H24:O24 R24:BO24 AA25:BO25 H25:N29 AA26:AB28 P27:Z27 S28:Z28 AO28:BO28 AK28:AK33 AM28:AM34 O29:W29 AO29:AO35 AP29:AQ36 AS29:BO36 AR29:AR37 H30:W31 H32:Y32 AJ32 AF33:AJ33 H33:Z35 AD34:AL34 AB35:AN35 H36:AA36 AF36:AO36 H37:AQ37 AS37:AV39 AW37:BO40 AG38:AR39 H38:Z43 AJ40:AV40 AH41:BO41 AN42:BO44 H44 H45:BO46">
+  <conditionalFormatting sqref="O5:BO5 I6 K6:BO6 K7 M7:M9 O7:BO9 J8:K8 H9 K9 AD10:BO10 H10:J16 L11:BO14 O15:BO17 L16:N16 H17:K17 M17:N17 N18:BO18 H18:L19 O19:BO19 AA20:BO20 H20:M21 O21:BO21 AA22:BO22 H22:N23 Q23 S23:BO23 H24:O24 R24:BO24 AA25:BO25 H25:N29 AA26:AB28 P27:Z27 S28:Z28 AO28:BO28 AK28:AK33 AM28:AM34 O29:W29 AO29:AO35 AP29:AQ36 AS29:BO36 AR29:AR37 H30:W31 H32:Y32 AJ32 AF33:AJ33 H33:Z35 AD34:AL34 AB35:AN35 H36:AA36 AF36:AO36 H37:AQ37 AS37:AV39 AW37:BO40 AG38:AR39 H38:Z43 AJ40:AV40 AH41:BO41 AN42:BO44 H44 H45:BO57">
     <cfRule type="expression" dxfId="63" priority="142">
       <formula>Plan</formula>
     </cfRule>
@@ -3893,14 +3997,14 @@
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c92308a8-1835-41e9-8926-04f7d96944eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="e356df2a-e0c9-4065-84cd-66458133e470"/>
-    <ds:schemaRef ds:uri="c92308a8-1835-41e9-8926-04f7d96944eb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>